<commit_message>
- doubled timestep in Test19 after reducing number of retained modes in SD to 0. - updated dependencies - removed extraneous args from calls to LAPACK_getrf and LAPACK_getrs (after updating library) - modified code to read SD summary file (follows mods in SD to output format)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@711 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="FAST v8.07.00" sheetId="4" r:id="rId1"/>
+    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -163,6 +162,63 @@
   </si>
   <si>
     <t>v1.01.02b-bjj</t>
+  </si>
+  <si>
+    <t>FEAMooring</t>
+  </si>
+  <si>
+    <t>IceFloe</t>
+  </si>
+  <si>
+    <t>IceDyn</t>
+  </si>
+  <si>
+    <t>x64</t>
+  </si>
+  <si>
+    <t>FAST v8.07.00</t>
+  </si>
+  <si>
+    <t>https://windsvn.nrel.gov/AeroDyn/trunk</t>
+  </si>
+  <si>
+    <t>https://windsvn.nrel.gov/FAST/branches/FAST_Registry</t>
+  </si>
+  <si>
+    <t>https://windsvn.nrel.gov/FAST/branches/BJonkman/Source/dependencies/FEAMooring</t>
+  </si>
+  <si>
+    <t>https://windsvn.nrel.gov/FAST/branches/FOA_modules/IceFloe</t>
+  </si>
+  <si>
+    <t>https://windsvn.nrel.gov/FAST/branches/FOA_modules/IceDyn</t>
+  </si>
+  <si>
+    <t>Source Code:</t>
+  </si>
+  <si>
+    <t>Executables:</t>
+  </si>
+  <si>
+    <t>Windows 32-bit</t>
+  </si>
+  <si>
+    <t>Windows 64-bit</t>
+  </si>
+  <si>
+    <t>Compiler</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>uses dummy MAP dll, thus does not run floating offshore systems</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>URL (released on web site)</t>
   </si>
 </sst>
 </file>
@@ -170,7 +226,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -197,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +272,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -230,14 +292,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -258,6 +320,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -560,10 +668,463 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="62" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="81.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <v>41823</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="14"/>
+      <c r="E27" s="20"/>
+      <c r="G27" s="14"/>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="14"/>
+      <c r="E28" s="20"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="14"/>
+      <c r="E29" s="20"/>
+      <c r="G29" s="14"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="14"/>
+      <c r="E30" s="20"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="14"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="14"/>
+      <c r="E31" s="20"/>
+      <c r="G31" s="14"/>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="14"/>
+      <c r="E32" s="20"/>
+      <c r="G32" s="14"/>
+      <c r="I32" s="14"/>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="14"/>
+      <c r="E33" s="20"/>
+      <c r="G33" s="14"/>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="14"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="14"/>
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="14"/>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="14"/>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="14"/>
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="17"/>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E40" s="17"/>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E42" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="C12:E12"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I25" r:id="rId1"/>
+    <hyperlink ref="I14" r:id="rId2"/>
+    <hyperlink ref="E17" r:id="rId3"/>
+    <hyperlink ref="E19" r:id="rId4"/>
+    <hyperlink ref="E21" r:id="rId5"/>
+    <hyperlink ref="E25" r:id="rId6"/>
+    <hyperlink ref="E14" r:id="rId7"/>
+    <hyperlink ref="E18" r:id="rId8"/>
+    <hyperlink ref="E20" r:id="rId9"/>
+    <hyperlink ref="I15" r:id="rId10"/>
+    <hyperlink ref="I16" r:id="rId11"/>
+    <hyperlink ref="I17" r:id="rId12"/>
+    <hyperlink ref="I19" r:id="rId13"/>
+    <hyperlink ref="I18" r:id="rId14"/>
+    <hyperlink ref="I20" r:id="rId15"/>
+    <hyperlink ref="I21" r:id="rId16"/>
+    <hyperlink ref="I26" r:id="rId17"/>
+    <hyperlink ref="E1" r:id="rId18"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,28 +1461,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
+ updated input files for FAST v8.8 and HD v2.1 + fixed bug in new HD conversion script + updated dependencies (including a few new source files for HD) + renamed conversion scripts for FAST because we aren't releasing v8.7.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@715 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>URL (released on web site)</t>
+  </si>
+  <si>
+    <t>1.01.00a-rrd</t>
   </si>
 </sst>
 </file>
@@ -335,9 +338,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -366,6 +366,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -671,7 +674,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +696,7 @@
         <v>53</v>
       </c>
       <c r="D1" s="13"/>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>32</v>
       </c>
       <c r="H1" s="13"/>
@@ -707,18 +710,18 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
@@ -745,14 +748,14 @@
       <c r="C9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="18"/>
       <c r="E9" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
@@ -761,38 +764,38 @@
       <c r="C10" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="18"/>
       <c r="F10" s="7"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19" t="s">
+      <c r="H10" s="18"/>
+      <c r="I10" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
+    <row r="11" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="27"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="18" t="s">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -823,14 +826,14 @@
         <v>7</v>
       </c>
       <c r="C14" s="14"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="21" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="20" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="21" t="s">
+      <c r="H14" s="18"/>
+      <c r="I14" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -839,12 +842,12 @@
         <v>9</v>
       </c>
       <c r="C15" s="14"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="21"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="7"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="21" t="s">
+      <c r="H15" s="18"/>
+      <c r="I15" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -853,12 +856,12 @@
         <v>10</v>
       </c>
       <c r="C16" s="14"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="21"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="7"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="21" t="s">
+      <c r="H16" s="18"/>
+      <c r="I16" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -867,14 +870,14 @@
         <v>8</v>
       </c>
       <c r="C17" s="14"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="21" t="s">
+      <c r="D17" s="18"/>
+      <c r="E17" s="20" t="s">
         <v>25</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="21" t="s">
+      <c r="H17" s="18"/>
+      <c r="I17" s="20" t="s">
         <v>54</v>
       </c>
     </row>
@@ -883,14 +886,14 @@
         <v>11</v>
       </c>
       <c r="C18" s="14"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="21" t="s">
+      <c r="D18" s="18"/>
+      <c r="E18" s="20" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="21" t="s">
+      <c r="H18" s="18"/>
+      <c r="I18" s="20" t="s">
         <v>40</v>
       </c>
     </row>
@@ -899,14 +902,14 @@
         <v>12</v>
       </c>
       <c r="C19" s="14"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="21" t="s">
+      <c r="D19" s="18"/>
+      <c r="E19" s="20" t="s">
         <v>27</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="21" t="s">
+      <c r="H19" s="18"/>
+      <c r="I19" s="20" t="s">
         <v>39</v>
       </c>
     </row>
@@ -914,15 +917,19 @@
       <c r="B20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="21" t="s">
+      <c r="C20" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="18">
+        <v>41802</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="21" t="s">
+      <c r="H20" s="18"/>
+      <c r="I20" s="20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -931,14 +938,14 @@
         <v>14</v>
       </c>
       <c r="C21" s="14"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="21" t="s">
+      <c r="D21" s="18"/>
+      <c r="E21" s="20" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="21" t="s">
+      <c r="H21" s="18"/>
+      <c r="I21" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -947,12 +954,12 @@
         <v>49</v>
       </c>
       <c r="C22" s="14"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="21"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="7"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="21" t="s">
+      <c r="H22" s="18"/>
+      <c r="I22" s="20" t="s">
         <v>56</v>
       </c>
     </row>
@@ -961,12 +968,12 @@
         <v>50</v>
       </c>
       <c r="C23" s="14"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="21"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="7"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="21" t="s">
+      <c r="H23" s="18"/>
+      <c r="I23" s="20" t="s">
         <v>57</v>
       </c>
     </row>
@@ -975,12 +982,12 @@
         <v>51</v>
       </c>
       <c r="C24" s="14"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="21"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="7"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="21" t="s">
+      <c r="H24" s="18"/>
+      <c r="I24" s="20" t="s">
         <v>58</v>
       </c>
     </row>
@@ -989,14 +996,14 @@
         <v>15</v>
       </c>
       <c r="C25" s="14"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="21" t="s">
+      <c r="D25" s="18"/>
+      <c r="E25" s="20" t="s">
         <v>30</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="21" t="s">
+      <c r="H25" s="18"/>
+      <c r="I25" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1005,76 +1012,76 @@
         <v>0</v>
       </c>
       <c r="C26" s="14"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
       <c r="F26" s="7"/>
       <c r="G26" s="14"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="21" t="s">
+      <c r="H26" s="18"/>
+      <c r="I26" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C27" s="14"/>
-      <c r="E27" s="20"/>
+      <c r="E27" s="19"/>
       <c r="G27" s="14"/>
       <c r="I27" s="14"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C28" s="14"/>
-      <c r="E28" s="20"/>
+      <c r="E28" s="19"/>
       <c r="G28" s="14"/>
       <c r="I28" s="14"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C29" s="14"/>
-      <c r="E29" s="20"/>
+      <c r="E29" s="19"/>
       <c r="G29" s="14"/>
       <c r="I29" s="14"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C30" s="14"/>
-      <c r="E30" s="20"/>
+      <c r="E30" s="19"/>
       <c r="G30" s="14"/>
       <c r="I30" s="14"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C31" s="14"/>
-      <c r="E31" s="20"/>
+      <c r="E31" s="19"/>
       <c r="G31" s="14"/>
       <c r="I31" s="14"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C32" s="14"/>
-      <c r="E32" s="20"/>
+      <c r="E32" s="19"/>
       <c r="G32" s="14"/>
       <c r="I32" s="14"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="14"/>
-      <c r="E33" s="20"/>
+      <c r="E33" s="19"/>
       <c r="G33" s="14"/>
       <c r="I33" s="14"/>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="14"/>
-      <c r="E34" s="20"/>
+      <c r="E34" s="19"/>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="14"/>
-      <c r="E35" s="20"/>
+      <c r="E35" s="19"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="14"/>
-      <c r="E36" s="20"/>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="14"/>
-      <c r="E37" s="20"/>
+      <c r="E37" s="19"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="14"/>
-      <c r="E38" s="20"/>
+      <c r="E38" s="19"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E39" s="17"/>
@@ -1124,7 +1131,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added switch to disable DWM made ValidateModeShapeCoeffs check a little less restrictive. Now instead of sum < 0.001, I check that it is < 0.0015
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@772 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>http://wind.nrel.gov/designcodes/simulators/FAST8/</t>
+  </si>
+  <si>
+    <t>Rev 474</t>
+  </si>
+  <si>
+    <t>v2.01.01c</t>
   </si>
 </sst>
 </file>
@@ -746,7 +752,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +764,7 @@
     <col min="5" max="5" width="62" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="81.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="20.28515625" customWidth="1"/>
@@ -1040,9 +1046,15 @@
         <v>27</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="G19" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="18">
+        <v>41820</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>91</v>
+      </c>
       <c r="J19" s="20" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
+ updated HD and SD input files based on new templates. updated main FAST input file with v8.9. + changed SD and HD locations for BJJ development to trunk
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@786 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
   </bookViews>
   <sheets>
-    <sheet name="FAST v8.08.00" sheetId="4" r:id="rId1"/>
-    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId2"/>
+    <sheet name="FAST v8.09.00" sheetId="5" r:id="rId1"/>
+    <sheet name="FAST v8.08.00" sheetId="4" r:id="rId2"/>
+    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="102">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -269,15 +270,6 @@
     <t>Tag</t>
   </si>
   <si>
-    <t>Rev 243</t>
-  </si>
-  <si>
-    <t>Rev 113</t>
-  </si>
-  <si>
-    <t>Rev 114</t>
-  </si>
-  <si>
     <t>Rev 59</t>
   </si>
   <si>
@@ -287,10 +279,49 @@
     <t>http://wind.nrel.gov/designcodes/simulators/FAST8/</t>
   </si>
   <si>
-    <t>Rev 474</t>
-  </si>
-  <si>
     <t>v2.01.01c</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/FAST8/</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/Aerodyn-Alpha</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/InflowWind-Alpha</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/HydroDyn</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/SubDyn</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/MAP/</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/IceFloe</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/NWTC_Library/</t>
+  </si>
+  <si>
+    <t>v1.01.00a</t>
+  </si>
+  <si>
+    <t>https://windsvn.nrel.gov/HydroDyn/trunk</t>
+  </si>
+  <si>
+    <t>https://wind-dev.nrel.gov/svn/SubDyn/trunk</t>
+  </si>
+  <si>
+    <t>https://wind-dev.nrel.gov/svn/SubDyn/branches/v1.00.00-rrd</t>
+  </si>
+  <si>
+    <t>v2.03.02</t>
+  </si>
+  <si>
+    <t>v2.00.01c-bjj</t>
   </si>
 </sst>
 </file>
@@ -752,7 +783,537 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="62" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="81.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <v>41822</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="18">
+        <v>41912</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="14">
+        <v>120</v>
+      </c>
+      <c r="H17" s="18">
+        <v>41906</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="18">
+        <v>41820</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="18">
+        <v>41912</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="18">
+        <v>41912</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="18">
+        <v>41703</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="18">
+        <v>41821</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="18">
+        <v>41820</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="18">
+        <v>41820</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="18">
+        <v>41820</v>
+      </c>
+      <c r="E24" s="32"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="18">
+        <v>41899</v>
+      </c>
+      <c r="E26" s="32"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="14"/>
+      <c r="E27" s="19"/>
+      <c r="G27" s="14"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="14"/>
+      <c r="E28" s="19"/>
+      <c r="G28" s="14"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="14"/>
+      <c r="E29" s="19"/>
+      <c r="G29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="14"/>
+      <c r="E30" s="19"/>
+      <c r="G30" s="14"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="14"/>
+      <c r="E31" s="19"/>
+      <c r="G31" s="14"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="14"/>
+      <c r="E32" s="19"/>
+      <c r="G32" s="14"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="14"/>
+      <c r="E33" s="19"/>
+      <c r="G33" s="14"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="14"/>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="14"/>
+      <c r="E35" s="19"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="14"/>
+      <c r="E36" s="19"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="14"/>
+      <c r="E37" s="19"/>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="14"/>
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="E39" s="17"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="E40" s="17"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="E42" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="G12:J12"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J25" r:id="rId1"/>
+    <hyperlink ref="J14" r:id="rId2"/>
+    <hyperlink ref="E16" r:id="rId3"/>
+    <hyperlink ref="E19" r:id="rId4"/>
+    <hyperlink ref="E21" r:id="rId5"/>
+    <hyperlink ref="E25" r:id="rId6"/>
+    <hyperlink ref="E14" r:id="rId7"/>
+    <hyperlink ref="E17" r:id="rId8"/>
+    <hyperlink ref="E20" r:id="rId9"/>
+    <hyperlink ref="J15" r:id="rId10"/>
+    <hyperlink ref="J18" r:id="rId11"/>
+    <hyperlink ref="J16" r:id="rId12"/>
+    <hyperlink ref="J19" r:id="rId13"/>
+    <hyperlink ref="J17" r:id="rId14"/>
+    <hyperlink ref="J20" r:id="rId15"/>
+    <hyperlink ref="J21" r:id="rId16"/>
+    <hyperlink ref="J26" r:id="rId17"/>
+    <hyperlink ref="E1" r:id="rId18"/>
+    <hyperlink ref="E23" r:id="rId19"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J42"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +1485,7 @@
         <v>41820</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="14">
@@ -973,8 +1534,8 @@
         <v>25</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="14" t="s">
-        <v>85</v>
+      <c r="G16" s="14">
+        <v>113</v>
       </c>
       <c r="H16" s="18">
         <v>41821</v>
@@ -1000,8 +1561,8 @@
         <v>34</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="14" t="s">
-        <v>86</v>
+      <c r="G17" s="14">
+        <v>114</v>
       </c>
       <c r="H17" s="18">
         <v>41821</v>
@@ -1046,14 +1607,14 @@
         <v>27</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="14" t="s">
-        <v>90</v>
+      <c r="G19" s="14">
+        <v>474</v>
       </c>
       <c r="H19" s="18">
         <v>41820</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J19" s="20" t="s">
         <v>39</v>
@@ -1073,11 +1634,17 @@
         <v>37</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="G20" s="14">
+        <v>315</v>
+      </c>
+      <c r="H20" s="18">
+        <v>41821</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>96</v>
+      </c>
       <c r="J20" s="20" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1094,8 +1661,8 @@
         <v>28</v>
       </c>
       <c r="F21" s="7"/>
-      <c r="G21" s="14" t="s">
-        <v>87</v>
+      <c r="G21" s="14">
+        <v>59</v>
       </c>
       <c r="H21" s="18">
         <v>41821</v>
@@ -1118,7 +1685,7 @@
       <c r="E22" s="32"/>
       <c r="F22" s="7"/>
       <c r="G22" s="30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
@@ -1141,7 +1708,7 @@
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
@@ -1162,7 +1729,7 @@
       <c r="E24" s="32"/>
       <c r="F24" s="7"/>
       <c r="G24" s="30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
@@ -1184,8 +1751,8 @@
         <v>30</v>
       </c>
       <c r="F25" s="7"/>
-      <c r="G25" s="14" t="s">
-        <v>84</v>
+      <c r="G25" s="14">
+        <v>243</v>
       </c>
       <c r="H25" s="18">
         <v>41821</v>
@@ -1207,10 +1774,10 @@
       <c r="D26" s="18">
         <v>41808</v>
       </c>
-      <c r="E26" s="19"/>
+      <c r="E26" s="32"/>
       <c r="F26" s="7"/>
       <c r="G26" s="30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H26" s="30"/>
       <c r="I26" s="30"/>
@@ -1324,7 +1891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>

</xml_diff>

<commit_message>
+ updated dependencies, adding first round of Andy's source files for next week's release + updated FAST version number
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@787 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="106">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -322,6 +322,18 @@
   </si>
   <si>
     <t>v2.00.01c-bjj</t>
+  </si>
+  <si>
+    <t>v2.04.00a-bjj</t>
+  </si>
+  <si>
+    <t>v1.01.07a-bjj</t>
+  </si>
+  <si>
+    <t>v14.03.00a-bjj</t>
+  </si>
+  <si>
+    <t>v8.09.00a-bjj</t>
   </si>
 </sst>
 </file>
@@ -783,7 +795,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +829,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="1">
-        <v>41822</v>
+        <v>41912</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -948,8 +960,12 @@
       <c r="B14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="18"/>
+      <c r="C14" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="18">
+        <v>41912</v>
+      </c>
       <c r="E14" s="20" t="s">
         <v>88</v>
       </c>
@@ -965,8 +981,12 @@
       <c r="B15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="18"/>
+      <c r="C15" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="18">
+        <v>41912</v>
+      </c>
       <c r="E15" s="32"/>
       <c r="F15" s="7"/>
       <c r="G15" s="30"/>
@@ -980,8 +1000,12 @@
       <c r="B16" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="18">
+        <v>41912</v>
+      </c>
       <c r="E16" s="20" t="s">
         <v>89</v>
       </c>
@@ -1013,7 +1037,7 @@
       <c r="H17" s="18">
         <v>41906</v>
       </c>
-      <c r="I17" s="18"/>
+      <c r="I17" s="31"/>
       <c r="J17" s="20" t="s">
         <v>40</v>
       </c>
@@ -1168,14 +1192,22 @@
       <c r="B25" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="18"/>
+      <c r="C25" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="18">
+        <v>41912</v>
+      </c>
       <c r="E25" s="20" t="s">
         <v>95</v>
       </c>
       <c r="F25" s="7"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="18"/>
+      <c r="G25" s="14">
+        <v>261</v>
+      </c>
+      <c r="H25" s="18">
+        <v>41908</v>
+      </c>
       <c r="I25" s="18"/>
       <c r="J25" s="20" t="s">
         <v>22</v>
@@ -1313,7 +1345,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
+ updated template file HD (removed extra comment) and updated CertTest input files + changed version number initials for HD in readme file
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@793 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="108">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>v8.09.00a-bjj</t>
+  </si>
+  <si>
+    <t>v1.01.01a-rrd</t>
+  </si>
+  <si>
+    <t>v2.02.00a-adp</t>
   </si>
 </sst>
 </file>
@@ -795,7 +801,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1071,9 @@
       <c r="B19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="14"/>
+      <c r="C19" s="14" t="s">
+        <v>107</v>
+      </c>
       <c r="D19" s="18">
         <v>41912</v>
       </c>
@@ -1083,6 +1091,9 @@
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>13</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="D20" s="18">
         <v>41912</v>

</xml_diff>

<commit_message>
+ updated with Andy P's latest HD changes
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@794 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -340,6 +340,15 @@
   </si>
   <si>
     <t>v2.02.00a-adp</t>
+  </si>
+  <si>
+    <t>v0.97.01a-mdm</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Didn't release or tag new version of InflowWind. Only difference between this version and FAST v8.08 release is location/name of registry files, which we updated in FAST.</t>
   </si>
 </sst>
 </file>
@@ -413,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -494,6 +503,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -800,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +826,7 @@
     <col min="6" max="6" width="8.42578125" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="81.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="20.28515625" customWidth="1"/>
   </cols>
@@ -835,7 +847,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="1">
-        <v>41912</v>
+        <v>41918</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1016,9 +1028,15 @@
         <v>89</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="G16" s="14">
+        <v>162</v>
+      </c>
+      <c r="H16" s="18">
+        <v>41915</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>104</v>
+      </c>
       <c r="J16" s="20" t="s">
         <v>53</v>
       </c>
@@ -1043,7 +1061,9 @@
       <c r="H17" s="18">
         <v>41906</v>
       </c>
-      <c r="I17" s="31"/>
+      <c r="I17" s="31" t="s">
+        <v>67</v>
+      </c>
       <c r="J17" s="20" t="s">
         <v>40</v>
       </c>
@@ -1129,7 +1149,9 @@
       <c r="H21" s="18">
         <v>41821</v>
       </c>
-      <c r="I21" s="18"/>
+      <c r="I21" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="J21" s="20" t="s">
         <v>42</v>
       </c>
@@ -1219,7 +1241,9 @@
       <c r="H25" s="18">
         <v>41908</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="18" t="s">
+        <v>102</v>
+      </c>
       <c r="J25" s="20" t="s">
         <v>22</v>
       </c>
@@ -1258,16 +1282,28 @@
       <c r="J28" s="14"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
+        <v>109</v>
+      </c>
       <c r="C29" s="14"/>
       <c r="E29" s="19"/>
       <c r="G29" s="14"/>
       <c r="J29" s="14"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="14"/>
-      <c r="E30" s="19"/>
-      <c r="G30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C31" s="14"/>
@@ -1320,10 +1356,11 @@
       <c r="E42" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="G12:J12"/>
+    <mergeCell ref="C30:J30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J25" r:id="rId1"/>

</xml_diff>

<commit_message>
updated dependencies, recompiled, reran CertTest and updated results (using updated test 19 and 25 HD input files from Jason Jonkman)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@800 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="111">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -813,7 +813,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,9 +988,15 @@
         <v>88</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="G14" s="14">
+        <v>801</v>
+      </c>
+      <c r="H14" s="18">
+        <v>41918</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>105</v>
+      </c>
       <c r="J14" s="20" t="s">
         <v>23</v>
       </c>
@@ -1101,8 +1107,12 @@
         <v>91</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="18"/>
+      <c r="G19" s="14">
+        <v>563</v>
+      </c>
+      <c r="H19" s="18">
+        <v>41918</v>
+      </c>
       <c r="I19" s="18"/>
       <c r="J19" s="20" t="s">
         <v>97</v>
@@ -1122,8 +1132,12 @@
         <v>92</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="18"/>
+      <c r="G20" s="14">
+        <v>332</v>
+      </c>
+      <c r="H20" s="18">
+        <v>41915</v>
+      </c>
       <c r="I20" s="18"/>
       <c r="J20" s="20" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
+ added HSSBrTrq + updated Simulink code to be a little more general; ;hooks for allowing inputs at t=0, though I'd disabled this feature for the time being (causes direct feed-through, which may cause other headaches) + changed DISCON dll suffix to x64 instead of win64 (so I can use $(PlatformName) in VS) + moved MAP and FEAM path locations + updated dependencies
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@946 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
+    <workbookView xWindow="240" yWindow="348" windowWidth="11808" windowHeight="5448"/>
   </bookViews>
   <sheets>
-    <sheet name="FAST v8.09.00" sheetId="5" r:id="rId1"/>
-    <sheet name="FAST v8.08.00" sheetId="4" r:id="rId2"/>
-    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId3"/>
+    <sheet name="FAST v8.10.00" sheetId="6" r:id="rId1"/>
+    <sheet name="FAST v8.09.00" sheetId="5" r:id="rId2"/>
+    <sheet name="FAST v8.08.00" sheetId="4" r:id="rId3"/>
+    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="148">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -349,6 +351,117 @@
   </si>
   <si>
     <t>Didn't release or tag new version of InflowWind. Only difference between this version and FAST v8.08 release is location/name of registry files, which we updated in FAST.</t>
+  </si>
+  <si>
+    <t>FAST v8.09.00</t>
+  </si>
+  <si>
+    <t>FAST v8.10.00</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/FAST8</t>
+  </si>
+  <si>
+    <t>1.10.0rc</t>
+  </si>
+  <si>
+    <t>v8.10.00a-bjj</t>
+  </si>
+  <si>
+    <t>MoorDyn</t>
+  </si>
+  <si>
+    <t>TMD</t>
+  </si>
+  <si>
+    <t>MATLAB 32-bit mex</t>
+  </si>
+  <si>
+    <t>MATLAB 64-bit mex</t>
+  </si>
+  <si>
+    <t>Visual Studio Community 2013 Update 4 (v120) [Win32]</t>
+  </si>
+  <si>
+    <t>Visual Studio Community 2013 Update 4 (v120) [x64]</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/TMD</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/FEAMooring</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/IceDyn</t>
+  </si>
+  <si>
+    <t>Git URL</t>
+  </si>
+  <si>
+    <t>mexw32</t>
+  </si>
+  <si>
+    <t>mexw64</t>
+  </si>
+  <si>
+    <t>Windows Executables:</t>
+  </si>
+  <si>
+    <t>v1.00.00-wgl</t>
+  </si>
+  <si>
+    <t>https://windsvn.nrel.gov/FAST/branches/FOA_modules/TMD</t>
+  </si>
+  <si>
+    <t>v1.10.0rc</t>
+  </si>
+  <si>
+    <t>v2.05.00</t>
+  </si>
+  <si>
+    <t>v2.05.02a-bjj</t>
+  </si>
+  <si>
+    <t>https://github.com/NREL/FEAMooring/branches/nrel_current</t>
+  </si>
+  <si>
+    <t>v1.01.00-yhb</t>
+  </si>
+  <si>
+    <t>https://github.com/matterhall/MoorDynF</t>
+  </si>
+  <si>
+    <t>14.03.01a-bjj</t>
+  </si>
+  <si>
+    <t>Rev</t>
+  </si>
+  <si>
+    <t>v2.02.01c-gjh</t>
+  </si>
+  <si>
+    <t>2.02.01c</t>
+  </si>
+  <si>
+    <t>v1.01.02a-rrd</t>
+  </si>
+  <si>
+    <t>v1.01.00-by</t>
+  </si>
+  <si>
+    <t>v2.01.00a-bjj</t>
+  </si>
+  <si>
+    <t>v1.01.02a</t>
+  </si>
+  <si>
+    <t>v2.01.00a</t>
+  </si>
+  <si>
+    <t>v14.03.01a-bjj</t>
+  </si>
+  <si>
+    <t>https://windsvn.nrel.gov/FAST/branches/FOA_modules/FEAMooring</t>
   </si>
 </sst>
 </file>
@@ -422,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -501,6 +614,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="1" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -810,117 +933,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="62" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="81.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="29" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1">
-        <v>41918</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
-        <v>59</v>
+      <c r="D2" s="1">
+        <v>42094</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>18</v>
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="14"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="14"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
-      <c r="J10" s="18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="25"/>
       <c r="D11" s="26"/>
       <c r="E11" s="27"/>
@@ -930,24 +1088,25 @@
       <c r="I11" s="26"/>
       <c r="J11" s="27"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
         <v>65</v>
       </c>
@@ -962,7 +1121,7 @@
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="3" t="s">
-        <v>5</v>
+        <v>138</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>6</v>
@@ -973,44 +1132,37 @@
       <c r="J13" s="15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>105</v>
+      <c r="C14" s="33" t="s">
+        <v>115</v>
       </c>
       <c r="D14" s="18">
-        <v>41912</v>
+        <v>42094</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>88</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="14">
-        <v>801</v>
-      </c>
-      <c r="H14" s="18">
-        <v>41918</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>105</v>
-      </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
       <c r="J14" s="20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="18">
-        <v>41912</v>
-      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="32"/>
       <c r="F15" s="7"/>
       <c r="G15" s="30"/>
@@ -1020,70 +1172,66 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>104</v>
+      <c r="C16" s="33" t="s">
+        <v>137</v>
       </c>
       <c r="D16" s="18">
-        <v>41912</v>
+        <v>42076</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>89</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="14">
-        <v>162</v>
+      <c r="G16" s="33">
+        <v>177</v>
       </c>
       <c r="H16" s="18">
-        <v>41915</v>
+        <v>42076</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="J16" s="20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>101</v>
+      <c r="C17" s="33" t="s">
+        <v>143</v>
       </c>
       <c r="D17" s="18">
-        <v>41912</v>
+        <v>42076</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>90</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="14">
-        <v>120</v>
+      <c r="G17" s="33">
+        <v>147</v>
       </c>
       <c r="H17" s="18">
-        <v>41906</v>
-      </c>
-      <c r="I17" s="31" t="s">
-        <v>67</v>
+        <v>42076</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="J17" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="18">
-        <v>41820</v>
-      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="32"/>
       <c r="F18" s="7"/>
       <c r="G18" s="30"/>
@@ -1093,7 +1241,647 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="18">
+        <v>42074</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="33"/>
+      <c r="J19" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="18">
+        <v>42072</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="33">
+        <v>607</v>
+      </c>
+      <c r="H20" s="18">
+        <v>42074</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="18">
+        <v>42062</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="33">
+        <v>344</v>
+      </c>
+      <c r="H21" s="18">
+        <v>42076</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="18">
+        <v>42073</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="33">
+        <v>108</v>
+      </c>
+      <c r="H22" s="18">
+        <v>42075</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" s="34"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="18">
+        <v>41987</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="33">
+        <v>943</v>
+      </c>
+      <c r="H23" s="18">
+        <v>42076</v>
+      </c>
+      <c r="I23" s="31"/>
+      <c r="J23" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="K23" s="34" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="32"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="18">
+        <v>41820</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="33">
+        <v>906</v>
+      </c>
+      <c r="H25" s="18">
+        <v>42040</v>
+      </c>
+      <c r="I25" s="31"/>
+      <c r="J25" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="18">
+        <v>42060</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="33">
+        <v>295</v>
+      </c>
+      <c r="H27" s="18">
+        <v>42075</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="18">
+        <v>42018</v>
+      </c>
+      <c r="E28" s="32"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="33">
+        <v>866</v>
+      </c>
+      <c r="H28" s="18">
+        <v>42020</v>
+      </c>
+      <c r="I28" s="30"/>
+      <c r="J28" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="33"/>
+      <c r="E29" s="19"/>
+      <c r="G29" s="33"/>
+      <c r="J29" s="33"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="33"/>
+      <c r="E30" s="19"/>
+      <c r="G30" s="33"/>
+      <c r="J30" s="33"/>
+    </row>
+    <row r="31" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C33" s="33"/>
+      <c r="E33" s="19"/>
+      <c r="G33" s="33"/>
+      <c r="J33" s="33"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C34" s="33"/>
+      <c r="E34" s="19"/>
+      <c r="G34" s="33"/>
+      <c r="J34" s="33"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="33"/>
+      <c r="E35" s="19"/>
+      <c r="G35" s="33"/>
+      <c r="J35" s="33"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C36" s="33"/>
+      <c r="E36" s="19"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C37" s="33"/>
+      <c r="E37" s="19"/>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C38" s="33"/>
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C39" s="33"/>
+      <c r="E39" s="19"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C40" s="33"/>
+      <c r="E40" s="19"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E42" s="17"/>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E43" s="17"/>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E44" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="B32:K32"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J27" r:id="rId1"/>
+    <hyperlink ref="J14" r:id="rId2"/>
+    <hyperlink ref="E16" r:id="rId3"/>
+    <hyperlink ref="E20" r:id="rId4"/>
+    <hyperlink ref="E22" r:id="rId5"/>
+    <hyperlink ref="E27" r:id="rId6"/>
+    <hyperlink ref="E14" r:id="rId7"/>
+    <hyperlink ref="E17" r:id="rId8"/>
+    <hyperlink ref="E21" r:id="rId9"/>
+    <hyperlink ref="J15" r:id="rId10"/>
+    <hyperlink ref="J18" r:id="rId11"/>
+    <hyperlink ref="J16" r:id="rId12"/>
+    <hyperlink ref="J20" r:id="rId13"/>
+    <hyperlink ref="J17" r:id="rId14"/>
+    <hyperlink ref="J21" r:id="rId15"/>
+    <hyperlink ref="J28" r:id="rId16"/>
+    <hyperlink ref="E1" r:id="rId17"/>
+    <hyperlink ref="E25" r:id="rId18"/>
+    <hyperlink ref="E19" r:id="rId19"/>
+    <hyperlink ref="E23" r:id="rId20"/>
+    <hyperlink ref="E26" r:id="rId21"/>
+    <hyperlink ref="J19" r:id="rId22"/>
+    <hyperlink ref="J22" r:id="rId23"/>
+    <hyperlink ref="K23" r:id="rId24"/>
+    <hyperlink ref="K24" r:id="rId25"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="62" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="81.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <v>41918</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="18">
+        <v>41912</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="14">
+        <v>801</v>
+      </c>
+      <c r="H14" s="18">
+        <v>41918</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="18">
+        <v>41912</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="18">
+        <v>41912</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="14">
+        <v>162</v>
+      </c>
+      <c r="H16" s="18">
+        <v>41915</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="18">
+        <v>41912</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="14">
+        <v>120</v>
+      </c>
+      <c r="H17" s="18">
+        <v>41906</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="18">
+        <v>41820</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
         <v>12</v>
       </c>
@@ -1118,7 +1906,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
         <v>13</v>
       </c>
@@ -1143,7 +1931,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
         <v>14</v>
       </c>
@@ -1170,7 +1958,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
         <v>49</v>
       </c>
@@ -1191,7 +1979,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
         <v>50</v>
       </c>
@@ -1214,7 +2002,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
         <v>51</v>
       </c>
@@ -1235,7 +2023,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
         <v>15</v>
       </c>
@@ -1262,7 +2050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
         <v>0</v>
       </c>
@@ -1283,19 +2071,19 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C27" s="14"/>
       <c r="E27" s="19"/>
       <c r="G27" s="14"/>
       <c r="J27" s="14"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C28" s="14"/>
       <c r="E28" s="19"/>
       <c r="G28" s="14"/>
       <c r="J28" s="14"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="13" t="s">
         <v>109</v>
       </c>
@@ -1304,69 +2092,69 @@
       <c r="G29" s="14"/>
       <c r="J29" s="14"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C31" s="14"/>
       <c r="E31" s="19"/>
       <c r="G31" s="14"/>
       <c r="J31" s="14"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C32" s="14"/>
       <c r="E32" s="19"/>
       <c r="G32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" s="14"/>
       <c r="E33" s="19"/>
       <c r="G33" s="14"/>
       <c r="J33" s="14"/>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C34" s="14"/>
       <c r="E34" s="19"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C35" s="14"/>
       <c r="E35" s="19"/>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C36" s="14"/>
       <c r="E36" s="19"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C37" s="14"/>
       <c r="E37" s="19"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C38" s="14"/>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E39" s="17"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E40" s="17"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E41" s="17"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E42" s="17"/>
     </row>
   </sheetData>
@@ -1402,7 +2190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
@@ -1410,22 +2198,22 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="14" customWidth="1"/>
     <col min="5" max="5" width="62" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="81.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="81.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>75</v>
       </c>
@@ -1436,7 +2224,7 @@
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1444,22 +2232,22 @@
         <v>41822</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="23"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="16"/>
       <c r="C8" s="16" t="s">
         <v>1</v>
@@ -1478,7 +2266,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
         <v>60</v>
       </c>
@@ -1495,7 +2283,7 @@
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
         <v>61</v>
       </c>
@@ -1514,7 +2302,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="25"/>
       <c r="D11" s="26"/>
       <c r="E11" s="27"/>
@@ -1524,24 +2312,24 @@
       <c r="I11" s="26"/>
       <c r="J11" s="27"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
         <v>65</v>
       </c>
@@ -1568,7 +2356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
         <v>7</v>
       </c>
@@ -1595,7 +2383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
         <v>9</v>
       </c>
@@ -1614,7 +2402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="13" t="s">
         <v>8</v>
       </c>
@@ -1641,7 +2429,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
         <v>11</v>
       </c>
@@ -1668,7 +2456,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
         <v>10</v>
       </c>
@@ -1687,7 +2475,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
         <v>12</v>
       </c>
@@ -1714,7 +2502,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
         <v>13</v>
       </c>
@@ -1741,7 +2529,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
         <v>14</v>
       </c>
@@ -1766,7 +2554,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
         <v>49</v>
       </c>
@@ -1787,7 +2575,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
         <v>50</v>
       </c>
@@ -1810,7 +2598,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
         <v>51</v>
       </c>
@@ -1831,7 +2619,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
         <v>15</v>
       </c>
@@ -1858,7 +2646,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
         <v>0</v>
       </c>
@@ -1879,78 +2667,78 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C27" s="14"/>
       <c r="E27" s="19"/>
       <c r="G27" s="14"/>
       <c r="J27" s="14"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C28" s="14"/>
       <c r="E28" s="19"/>
       <c r="G28" s="14"/>
       <c r="J28" s="14"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C29" s="14"/>
       <c r="E29" s="19"/>
       <c r="G29" s="14"/>
       <c r="J29" s="14"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C30" s="14"/>
       <c r="E30" s="19"/>
       <c r="G30" s="14"/>
       <c r="J30" s="14"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C31" s="14"/>
       <c r="E31" s="19"/>
       <c r="G31" s="14"/>
       <c r="J31" s="14"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C32" s="14"/>
       <c r="E32" s="19"/>
       <c r="G32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" s="14"/>
       <c r="E33" s="19"/>
       <c r="G33" s="14"/>
       <c r="J33" s="14"/>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C34" s="14"/>
       <c r="E34" s="19"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C35" s="14"/>
       <c r="E35" s="19"/>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C36" s="14"/>
       <c r="E36" s="19"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C37" s="14"/>
       <c r="E37" s="19"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C38" s="14"/>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E39" s="17"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E40" s="17"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E41" s="17"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E42" s="17"/>
     </row>
   </sheetData>
@@ -1985,7 +2773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
@@ -1993,19 +2781,19 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="20.28515625" customWidth="1"/>
+    <col min="3" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2013,13 +2801,13 @@
         <v>41550</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -2027,7 +2815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
@@ -2062,12 +2850,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -2102,7 +2890,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2925,7 @@
         <v>41547</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>2</v>
       </c>
@@ -2170,7 +2958,7 @@
       </c>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -2182,7 +2970,7 @@
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
@@ -2197,7 +2985,7 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -2232,7 +3020,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -2267,7 +3055,7 @@
         <v>41547</v>
       </c>
     </row>
-    <row r="18" spans="2:12" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" s="9" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
bug fixes in ServoDyn and HydroDyn (now get same CertTest results)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@950 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -13,7 +13,6 @@
     <sheet name="FAST v8.03.02" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -935,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,7 +1254,13 @@
         <v>122</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="33"/>
+      <c r="G19" s="33">
+        <v>934</v>
+      </c>
+      <c r="H19" s="18">
+        <v>42074</v>
+      </c>
+      <c r="I19" s="31"/>
       <c r="J19" s="20" t="s">
         <v>130</v>
       </c>

</xml_diff>

<commit_message>
+ removed Crunch stuff from CertTest.bat + changed MAP to MAP++ in primary input file comments + updated documentation with JMJ comments + updated dependencies + updated version date
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@954 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -633,13 +633,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -947,7 +947,7 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,11 +989,11 @@
       <c r="B5" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -1103,18 +1103,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1382,10 +1382,10 @@
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="33">
-        <v>943</v>
+        <v>953</v>
       </c>
       <c r="H23" s="18">
-        <v>42076</v>
+        <v>42094</v>
       </c>
       <c r="I23" s="31"/>
       <c r="J23" s="20" t="s">
@@ -1402,7 +1402,7 @@
       <c r="C24" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="38">
         <v>42093</v>
       </c>
       <c r="E24" s="32"/>
@@ -1537,16 +1537,16 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" s="33"/>
@@ -1683,11 +1683,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -1763,18 +1763,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
@@ -2137,16 +2137,16 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C31" s="14"/>
@@ -2277,11 +2277,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -2357,18 +2357,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">

</xml_diff>

<commit_message>
+ ran CertTest and updated TstFiles with results + tweaked a few things in the ReadMe file
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@958 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="151">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t>b38fc19f74521811f3927cb964b7dacc99e7541c</t>
+  </si>
+  <si>
+    <t>MATLAB R2014b</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -628,6 +631,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -946,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,11 +995,11 @@
       <c r="B5" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -1066,8 +1072,9 @@
       <c r="E9" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="33" t="s">
+        <v>150</v>
+      </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -1083,8 +1090,9 @@
       <c r="E10" t="s">
         <v>121</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="33"/>
+      <c r="F10" s="38" t="s">
+        <v>150</v>
+      </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -1103,18 +1111,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1161,9 +1169,15 @@
         <v>88</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="G14" s="33">
+        <v>959</v>
+      </c>
+      <c r="H14" s="18">
+        <v>42094</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>115</v>
+      </c>
       <c r="J14" s="20" t="s">
         <v>23</v>
       </c>
@@ -1402,7 +1416,7 @@
       <c r="C24" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="39">
         <v>42093</v>
       </c>
       <c r="E24" s="32"/>
@@ -1537,16 +1551,16 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" s="33"/>
@@ -1683,11 +1697,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -1763,18 +1777,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
@@ -2137,16 +2151,16 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C31" s="14"/>
@@ -2277,11 +2291,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -2357,18 +2371,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">

</xml_diff>

<commit_message>
ServoDyn: added error checking on DLL_DT and added a delay for the DLL when DLL_DT > DT (when compiler directive is used) to provide linear ramps in commanded pitch instead of step changes (for BeamDyn) FAST: fixed serious index errors with the OrcaFlex integration. Fixed potential memory leak when the Jacobian was calculated and OrcaFlex used. + updated dependencies
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1127 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="240" yWindow="348" windowWidth="11808" windowHeight="5448"/>
   </bookViews>
   <sheets>
-    <sheet name="FAST v8.10.00" sheetId="6" r:id="rId1"/>
-    <sheet name="FAST v8.09.00" sheetId="5" r:id="rId2"/>
-    <sheet name="FAST v8.08.00" sheetId="4" r:id="rId3"/>
-    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId4"/>
+    <sheet name="FAST v8.12.00" sheetId="7" r:id="rId1"/>
+    <sheet name="FAST v8.10.00" sheetId="6" r:id="rId2"/>
+    <sheet name="FAST v8.09.00" sheetId="5" r:id="rId3"/>
+    <sheet name="FAST v8.08.00" sheetId="4" r:id="rId4"/>
+    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="160">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -470,6 +471,33 @@
   </si>
   <si>
     <t>MATLAB R2014b</t>
+  </si>
+  <si>
+    <t>AeroDyn 15</t>
+  </si>
+  <si>
+    <t>BeamDyn</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/BeamDyn</t>
+  </si>
+  <si>
+    <t>v8.12.00a-bjj</t>
+  </si>
+  <si>
+    <t>DWM</t>
+  </si>
+  <si>
+    <t>Intel(R) Visual Fortran Composer XE 2013 SP1 14.0.5.239 [IA-32]</t>
+  </si>
+  <si>
+    <t>Intel(R) Visual Fortran Composer XE 2013 SP1 14.0.5.239 [Intel(R)-64]</t>
+  </si>
+  <si>
+    <t>Visual Studio Community 2013 Update 4 (v120) 12.0.31101.00 [Win32]</t>
+  </si>
+  <si>
+    <t>Visual Studio Community 2013 Update 4 (v120) 12.0.31101.00 [x64]</t>
   </si>
 </sst>
 </file>
@@ -543,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -640,6 +668,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -950,10 +981,650 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" t="s">
+        <v>159</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K25" s="34"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="K26" s="34" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="40"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="40"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="40"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="40"/>
+      <c r="E32" s="19"/>
+      <c r="G32" s="40"/>
+      <c r="J32" s="40"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C33" s="40"/>
+      <c r="E33" s="19"/>
+      <c r="G33" s="40"/>
+      <c r="J33" s="40"/>
+    </row>
+    <row r="34" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C36" s="40"/>
+      <c r="E36" s="19"/>
+      <c r="G36" s="40"/>
+      <c r="J36" s="40"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C37" s="40"/>
+      <c r="E37" s="19"/>
+      <c r="G37" s="40"/>
+      <c r="J37" s="40"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C38" s="40"/>
+      <c r="E38" s="19"/>
+      <c r="G38" s="40"/>
+      <c r="J38" s="40"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C39" s="40"/>
+      <c r="E39" s="19"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C40" s="40"/>
+      <c r="E40" s="19"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C41" s="40"/>
+      <c r="E41" s="19"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C42" s="40"/>
+      <c r="E42" s="19"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C43" s="40"/>
+      <c r="E43" s="19"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E44" s="17"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E46" s="17"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E47" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="B35:K35"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J30" r:id="rId1"/>
+    <hyperlink ref="J14" r:id="rId2"/>
+    <hyperlink ref="E18" r:id="rId3"/>
+    <hyperlink ref="E23" r:id="rId4"/>
+    <hyperlink ref="E25" r:id="rId5"/>
+    <hyperlink ref="E30" r:id="rId6"/>
+    <hyperlink ref="E14" r:id="rId7"/>
+    <hyperlink ref="E20" r:id="rId8"/>
+    <hyperlink ref="E24" r:id="rId9"/>
+    <hyperlink ref="J15" r:id="rId10"/>
+    <hyperlink ref="J21" r:id="rId11"/>
+    <hyperlink ref="J18" r:id="rId12"/>
+    <hyperlink ref="J23" r:id="rId13"/>
+    <hyperlink ref="J20" r:id="rId14"/>
+    <hyperlink ref="J24" r:id="rId15"/>
+    <hyperlink ref="J31" r:id="rId16"/>
+    <hyperlink ref="E1" r:id="rId17"/>
+    <hyperlink ref="E28" r:id="rId18"/>
+    <hyperlink ref="E22" r:id="rId19"/>
+    <hyperlink ref="E26" r:id="rId20"/>
+    <hyperlink ref="E29" r:id="rId21"/>
+    <hyperlink ref="J22" r:id="rId22"/>
+    <hyperlink ref="J25" r:id="rId23"/>
+    <hyperlink ref="K26" r:id="rId24"/>
+    <hyperlink ref="K27" r:id="rId25"/>
+    <hyperlink ref="E16" r:id="rId26"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,11 +1666,11 @@
       <c r="B5" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -1111,18 +1782,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1551,16 +2222,16 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" s="33"/>
@@ -1651,7 +2322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
@@ -1697,11 +2368,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -1777,18 +2448,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
@@ -2151,16 +2822,16 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C31" s="14"/>
@@ -2245,7 +2916,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
@@ -2291,11 +2962,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -2371,18 +3042,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
@@ -2828,7 +3499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated version numbers in ED and SrvD; updated dependencies
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1143 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="169">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -428,9 +428,6 @@
     <t>v1.01.00-yhb</t>
   </si>
   <si>
-    <t>https://github.com/matterhall/MoorDynF</t>
-  </si>
-  <si>
     <t>Rev</t>
   </si>
   <si>
@@ -507,6 +504,27 @@
   </si>
   <si>
     <t>https://github.com/mattEhall/MoorDynF</t>
+  </si>
+  <si>
+    <t>v2.06.05a-bjj</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/Aerodyn14</t>
+  </si>
+  <si>
+    <t>http://nwtc.nrel.gov/InflowWind</t>
+  </si>
+  <si>
+    <t>https://windsvn.nrel.gov/InflowWind/branches/modularization2</t>
+  </si>
+  <si>
+    <t>v1.03.00a-bjj</t>
+  </si>
+  <si>
+    <t>v1.03.01a-bjj</t>
+  </si>
+  <si>
+    <t>v2.08.03</t>
   </si>
 </sst>
 </file>
@@ -992,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,7 +1094,7 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="40"/>
@@ -1093,7 +1111,7 @@
       </c>
       <c r="D8" s="18"/>
       <c r="E8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="40"/>
@@ -1110,10 +1128,10 @@
       </c>
       <c r="D9" s="18"/>
       <c r="E9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -1127,10 +1145,10 @@
       </c>
       <c r="D10" s="18"/>
       <c r="E10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -1178,7 +1196,7 @@
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>4</v>
@@ -1194,14 +1212,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>85</v>
-      </c>
       <c r="B14" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="20" t="s">
@@ -1219,8 +1234,12 @@
       <c r="B15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="18"/>
+      <c r="C15" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="18">
+        <v>42282</v>
+      </c>
       <c r="E15" s="32"/>
       <c r="F15" s="7"/>
       <c r="G15" s="30"/>
@@ -1231,16 +1250,13 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>85</v>
-      </c>
       <c r="B16" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="18"/>
       <c r="E16" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="40"/>
@@ -1248,12 +1264,9 @@
       <c r="I16" s="18"/>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>85</v>
-      </c>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="18"/>
@@ -1264,17 +1277,14 @@
       <c r="I17" s="18"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>85</v>
-      </c>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="18"/>
       <c r="E18" s="20" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="40"/>
@@ -1284,12 +1294,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>85</v>
-      </c>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="18"/>
@@ -1300,32 +1307,33 @@
       <c r="I19" s="18"/>
       <c r="J19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>85</v>
-      </c>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="18"/>
       <c r="E20" s="20" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="40"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
       <c r="J20" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="18"/>
+      <c r="C21" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="18">
+        <v>42282</v>
+      </c>
       <c r="E21" s="32"/>
       <c r="F21" s="7"/>
       <c r="G21" s="30"/>
@@ -1335,12 +1343,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
         <v>117</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D22" s="18">
         <v>42268</v>
@@ -1360,10 +1368,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>85</v>
-      </c>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
         <v>12</v>
       </c>
@@ -1380,10 +1385,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>85</v>
-      </c>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
         <v>13</v>
       </c>
@@ -1400,10 +1402,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>85</v>
-      </c>
+    <row r="25" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
         <v>14</v>
       </c>
@@ -1421,38 +1420,29 @@
       </c>
       <c r="K25" s="34"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="D26" s="18">
-        <v>42268</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="D26" s="18"/>
       <c r="E26" s="20" t="s">
         <v>123</v>
       </c>
       <c r="F26" s="7"/>
-      <c r="G26" s="40">
-        <v>1131</v>
-      </c>
-      <c r="H26" s="18">
-        <v>42268</v>
-      </c>
+      <c r="G26" s="40"/>
+      <c r="H26" s="18"/>
       <c r="I26" s="31"/>
       <c r="J26" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K26" s="34" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>85</v>
-      </c>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="13" t="s">
         <v>116</v>
       </c>
@@ -1465,10 +1455,10 @@
       <c r="I27" s="31"/>
       <c r="J27" s="20"/>
       <c r="K27" s="34" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="13" t="s">
         <v>50</v>
       </c>
@@ -1485,10 +1475,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>85</v>
-      </c>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="13" t="s">
         <v>51</v>
       </c>
@@ -1505,32 +1492,41 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>85</v>
-      </c>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" s="18">
+        <v>42282</v>
+      </c>
       <c r="E30" s="20" t="s">
         <v>95</v>
       </c>
       <c r="F30" s="7"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="18"/>
+      <c r="G30" s="40">
+        <v>344</v>
+      </c>
+      <c r="H30" s="18">
+        <v>42282</v>
+      </c>
       <c r="I30" s="18"/>
       <c r="J30" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="18"/>
+      <c r="C31" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="18">
+        <v>42279</v>
+      </c>
       <c r="E31" s="32"/>
       <c r="F31" s="7"/>
       <c r="G31" s="40"/>
@@ -1540,7 +1536,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C32" s="40"/>
       <c r="E32" s="19"/>
       <c r="G32" s="40"/>
@@ -1663,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1784,7 +1780,7 @@
         <v>120</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
@@ -1802,7 +1798,7 @@
         <v>121</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
@@ -1851,7 +1847,7 @@
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>4</v>
@@ -1898,7 +1894,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="18">
         <v>42094</v>
@@ -1917,7 +1913,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D16" s="18">
         <v>42076</v>
@@ -1933,7 +1929,7 @@
         <v>42076</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J16" s="20" t="s">
         <v>53</v>
@@ -1944,7 +1940,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" s="18">
         <v>42076</v>
@@ -1960,7 +1956,7 @@
         <v>42076</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J17" s="20" t="s">
         <v>40</v>
@@ -1971,7 +1967,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D18" s="18">
         <v>42094</v>
@@ -2015,7 +2011,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" s="18">
         <v>42088</v>
@@ -2031,7 +2027,7 @@
         <v>42088</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J20" s="20" t="s">
         <v>97</v>
@@ -2042,7 +2038,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D21" s="18">
         <v>42062</v>
@@ -2058,7 +2054,7 @@
         <v>42076</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J21" s="20" t="s">
         <v>98</v>
@@ -2114,7 +2110,7 @@
       </c>
       <c r="I23" s="31"/>
       <c r="J23" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K23" s="34" t="s">
         <v>134</v>
@@ -2125,7 +2121,7 @@
         <v>116</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D24" s="39">
         <v>42093</v>
@@ -2133,7 +2129,7 @@
       <c r="E24" s="32"/>
       <c r="F24" s="7"/>
       <c r="G24" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H24" s="18">
         <v>42093</v>
@@ -2141,7 +2137,7 @@
       <c r="I24" s="31"/>
       <c r="J24" s="20"/>
       <c r="K24" s="34" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -2174,7 +2170,7 @@
         <v>51</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D26" s="18">
         <v>42093</v>

</xml_diff>

<commit_message>
ran CertTest one last time (with Crunch) and updated TstFiles.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1158 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="204">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -1116,7 +1116,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1330,11 +1330,15 @@
         <v>181</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="40"/>
+      <c r="G14" s="40">
+        <v>1159</v>
+      </c>
       <c r="H14" s="18">
         <v>42284</v>
       </c>
-      <c r="I14" s="18"/>
+      <c r="I14" s="18" t="s">
+        <v>151</v>
+      </c>
       <c r="J14" s="20" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
+ added STATIC_DLL_LOAD preprocessor directive for OpenFOAM to load the DLL on program start regardless of if it is being used (problem with MPI task not making separate copies of the dynamically loaded library) + fixed IfW error handling when HAWC winds aren't read properly.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1160 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="204">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -1115,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1329,7 +1329,9 @@
       <c r="E14" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="G14" s="40">
         <v>1159</v>
       </c>

</xml_diff>

<commit_message>
-changed version date/number -updated copyright text -updated dependencies -modified text-file output to write single-precision numbers so that format statements work better with double-precision version of FAST.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1260 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="408" windowWidth="11808" windowHeight="5316"/>
+    <workbookView xWindow="240" yWindow="468" windowWidth="11808" windowHeight="5256"/>
   </bookViews>
   <sheets>
     <sheet name="FAST v8.15.00" sheetId="8" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="242">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -713,6 +713,39 @@
   </si>
   <si>
     <t>1.20.10</t>
+  </si>
+  <si>
+    <t>v1.02.00</t>
+  </si>
+  <si>
+    <t>Archive Released</t>
+  </si>
+  <si>
+    <t>v3.02.00a-bjj</t>
+  </si>
+  <si>
+    <t>v1.01.01</t>
+  </si>
+  <si>
+    <t>v2.01.03-yh</t>
+  </si>
+  <si>
+    <t>v14.05.00a-bjj</t>
+  </si>
+  <si>
+    <t>https://bitbucket.org/mmasciola/map-plus-plus/branch/master</t>
+  </si>
+  <si>
+    <t>v1.20.10</t>
+  </si>
+  <si>
+    <t>v1.03.00</t>
+  </si>
+  <si>
+    <t>v15.02.03</t>
+  </si>
+  <si>
+    <t>v1.01.03</t>
   </si>
 </sst>
 </file>
@@ -722,7 +755,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,8 +779,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -772,6 +812,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -782,11 +827,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -900,9 +946,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1204,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,7 +1268,7 @@
     <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="41" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="41" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5546875" style="41" bestFit="1" customWidth="1"/>
@@ -1375,7 +1428,7 @@
       <c r="J12" s="43"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
         <v>65</v>
       </c>
@@ -1388,7 +1441,9 @@
       <c r="E13" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="45" t="s">
+        <v>232</v>
+      </c>
       <c r="G13" s="3" t="s">
         <v>136</v>
       </c>
@@ -1455,19 +1510,17 @@
         <v>150</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="D16" s="18">
-        <v>42465</v>
+        <v>42471</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>226</v>
-      </c>
+      <c r="F16" s="7"/>
       <c r="G16" s="41">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="H16" s="18">
         <v>42465</v>
@@ -1484,13 +1537,19 @@
       <c r="B17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D17" s="18">
+        <v>42471</v>
+      </c>
       <c r="E17" s="20" t="s">
         <v>206</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="41"/>
+      <c r="G17" s="46">
+        <v>219</v>
+      </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="20" t="s">
@@ -1501,15 +1560,27 @@
       <c r="B18" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="D18" s="18">
+        <v>42471</v>
+      </c>
       <c r="E18" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="F18" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G18" s="41">
+        <v>223</v>
+      </c>
+      <c r="H18" s="18">
+        <v>42471</v>
+      </c>
+      <c r="I18" s="42" t="s">
+        <v>236</v>
+      </c>
       <c r="J18" s="20" t="s">
         <v>53</v>
       </c>
@@ -1518,13 +1589,23 @@
       <c r="B19" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="18"/>
+      <c r="C19" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="D19" s="18">
+        <v>42471</v>
+      </c>
       <c r="E19" s="32"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="42">
+        <v>223</v>
+      </c>
+      <c r="H19" s="18">
+        <v>42471</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>236</v>
+      </c>
       <c r="J19" s="20" t="s">
         <v>53</v>
       </c>
@@ -1538,7 +1619,9 @@
       <c r="E20" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7" t="s">
+        <v>221</v>
+      </c>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
       <c r="I20" s="31"/>
@@ -1550,15 +1633,27 @@
       <c r="B21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="18"/>
+      <c r="C21" s="41" t="s">
+        <v>233</v>
+      </c>
+      <c r="D21" s="18">
+        <v>42471</v>
+      </c>
       <c r="E21" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="F21" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G21" s="41">
+        <v>202</v>
+      </c>
+      <c r="H21" s="18">
+        <v>42471</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>233</v>
+      </c>
       <c r="J21" s="20" t="s">
         <v>161</v>
       </c>
@@ -1625,13 +1720,19 @@
       <c r="B24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="18"/>
+      <c r="C24" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" s="18">
+        <v>42444</v>
+      </c>
       <c r="E24" s="20" t="s">
         <v>210</v>
       </c>
       <c r="F24" s="7"/>
-      <c r="G24" s="41"/>
+      <c r="G24" s="46">
+        <v>670</v>
+      </c>
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
       <c r="J24" s="20" t="s">
@@ -1643,10 +1744,10 @@
         <v>165</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="D25" s="18">
-        <v>42444</v>
+        <v>42471</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>211</v>
@@ -1655,7 +1756,7 @@
         <v>226</v>
       </c>
       <c r="G25" s="41">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H25" s="18">
         <v>42468</v>
@@ -1671,15 +1772,27 @@
       <c r="B26" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="18"/>
+      <c r="C26" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="18">
+        <v>42471</v>
+      </c>
       <c r="E26" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="F26" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G26" s="41">
+        <v>368</v>
+      </c>
+      <c r="H26" s="18">
+        <v>42471</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>239</v>
+      </c>
       <c r="J26" s="20" t="s">
         <v>98</v>
       </c>
@@ -1691,33 +1804,53 @@
       <c r="C27" s="41" t="s">
         <v>230</v>
       </c>
-      <c r="D27" s="18"/>
+      <c r="D27" s="18">
+        <v>42471</v>
+      </c>
       <c r="E27" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
+      <c r="F27" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G27" s="41">
+        <v>132</v>
+      </c>
+      <c r="H27" s="18">
+        <v>42471</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>238</v>
+      </c>
       <c r="J27" s="20" t="s">
         <v>42</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>198</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="18"/>
+      <c r="C28" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="D28" s="18">
+        <v>42376</v>
+      </c>
       <c r="E28" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="18"/>
+      <c r="F28" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G28" s="41">
+        <v>1242</v>
+      </c>
+      <c r="H28" s="18">
+        <v>42469</v>
+      </c>
       <c r="I28" s="31"/>
       <c r="J28" s="20" t="s">
         <v>143</v>
@@ -1760,14 +1893,24 @@
       <c r="B30" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="D30" s="18">
+        <v>42377</v>
+      </c>
       <c r="E30" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="18"/>
+      <c r="F30" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="G30" s="41">
+        <v>1241</v>
+      </c>
+      <c r="H30" s="18">
+        <v>42469</v>
+      </c>
       <c r="I30" s="31"/>
       <c r="J30" s="20" t="s">
         <v>56</v>
@@ -1777,14 +1920,24 @@
       <c r="B31" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="18"/>
+      <c r="C31" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="D31" s="18">
+        <v>42377</v>
+      </c>
       <c r="E31" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="18"/>
+      <c r="F31" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="G31" s="41">
+        <v>1239</v>
+      </c>
+      <c r="H31" s="18">
+        <v>42469</v>
+      </c>
       <c r="I31" s="31"/>
       <c r="J31" s="20" t="s">
         <v>57</v>
@@ -1967,9 +2120,10 @@
     <hyperlink ref="J17" r:id="rId34"/>
     <hyperlink ref="K22" r:id="rId35"/>
     <hyperlink ref="K23" r:id="rId36"/>
+    <hyperlink ref="K27" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
 </worksheet>
 </file>
 
@@ -1978,7 +2132,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
- updated compile_FAST.bat and makefile so they successfully compile FAST - fixed ArcFiles.txt so it contains the AeroDyn 15 blade files and matlab conversion scripts; removed some unnecessary files - fixed typo in readme
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1271 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="468" windowWidth="11808" windowHeight="5256"/>
+    <workbookView xWindow="1776" yWindow="6660" windowWidth="11808" windowHeight="3588"/>
   </bookViews>
   <sheets>
     <sheet name="FAST v8.15.00" sheetId="8" r:id="rId1"/>
@@ -15,12 +15,11 @@
     <sheet name="FAST v8.03.02" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="245">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -746,6 +745,15 @@
   </si>
   <si>
     <t>v1.01.03</t>
+  </si>
+  <si>
+    <t>v8.15.00a-bjj</t>
+  </si>
+  <si>
+    <t>&lt;later&gt;</t>
+  </si>
+  <si>
+    <t>FAST v8.15.00</t>
   </si>
 </sst>
 </file>
@@ -755,7 +763,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,13 +789,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -814,6 +829,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
@@ -827,12 +847,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -940,22 +961,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1257,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1279,7 +1304,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>112</v>
+        <v>244</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="29" t="s">
@@ -1293,18 +1318,18 @@
         <v>19</v>
       </c>
       <c r="D2" s="1">
-        <v>42468</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -1414,18 +1439,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1441,7 +1466,7 @@
       <c r="E13" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="43" t="s">
         <v>232</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -1464,15 +1489,27 @@
       <c r="B14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="18"/>
+      <c r="C14" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="D14" s="18">
+        <v>42472</v>
+      </c>
       <c r="E14" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="F14" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="G14" s="41">
+        <v>1272</v>
+      </c>
+      <c r="H14" s="18">
+        <v>42473</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>242</v>
+      </c>
       <c r="J14" s="20" t="s">
         <v>23</v>
       </c>
@@ -1513,12 +1550,14 @@
         <v>241</v>
       </c>
       <c r="D16" s="18">
-        <v>42471</v>
+        <v>42472</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>226</v>
+      </c>
       <c r="G16" s="41">
         <v>816</v>
       </c>
@@ -1546,12 +1585,18 @@
       <c r="E17" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="46">
+      <c r="F17" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="G17" s="44">
         <v>219</v>
       </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="H17" s="18">
+        <v>42472</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>243</v>
+      </c>
       <c r="J17" s="20" t="s">
         <v>202</v>
       </c>
@@ -1729,12 +1774,18 @@
       <c r="E24" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="46">
+      <c r="F24" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="G24" s="44">
         <v>670</v>
       </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="H24" s="18">
+        <v>42471</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>243</v>
+      </c>
       <c r="J24" s="20" t="s">
         <v>97</v>
       </c>
@@ -2015,16 +2066,16 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="47"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C38" s="41"/>
@@ -2131,7 +2182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2174,11 +2225,11 @@
       <c r="B5" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -2288,18 +2339,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2884,16 +2935,16 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="47"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C38" s="40"/>
@@ -3041,11 +3092,11 @@
       <c r="B5" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -3157,18 +3208,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3597,16 +3648,16 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" s="33"/>
@@ -3743,11 +3794,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -3823,18 +3874,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
@@ -4197,16 +4248,16 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C31" s="14"/>
@@ -4337,11 +4388,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -4417,18 +4468,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">

</xml_diff>

<commit_message>
removed external inputs from glue code and placed them as external inputs in individual modules; removed unused variables; fixed bug in index in Linear_AD_InputSolve_IfW_dy(); changes RootName in FEAM init to append .FEAM in glue instead of module updated dependencies
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1299 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -7,19 +7,20 @@
     <workbookView xWindow="1776" yWindow="6660" windowWidth="11808" windowHeight="3588"/>
   </bookViews>
   <sheets>
-    <sheet name="FAST v8.15.00" sheetId="8" r:id="rId1"/>
-    <sheet name="FAST v8.12.00" sheetId="7" r:id="rId2"/>
-    <sheet name="FAST v8.10.00" sheetId="6" r:id="rId3"/>
-    <sheet name="FAST v8.09.00" sheetId="5" r:id="rId4"/>
-    <sheet name="FAST v8.08.00" sheetId="4" r:id="rId5"/>
-    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId6"/>
+    <sheet name="FAST v8.16.00" sheetId="9" r:id="rId1"/>
+    <sheet name="FAST v8.15.00" sheetId="8" r:id="rId2"/>
+    <sheet name="FAST v8.12.00" sheetId="7" r:id="rId3"/>
+    <sheet name="FAST v8.10.00" sheetId="6" r:id="rId4"/>
+    <sheet name="FAST v8.09.00" sheetId="5" r:id="rId5"/>
+    <sheet name="FAST v8.08.00" sheetId="4" r:id="rId6"/>
+    <sheet name="FAST v8.03.02" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="261">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -754,6 +755,54 @@
   </si>
   <si>
     <t>FAST v8.15.00</t>
+  </si>
+  <si>
+    <t>v8.16.00a-bjj</t>
+  </si>
+  <si>
+    <t>v3.02.00</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/FAST_Registry/</t>
+  </si>
+  <si>
+    <t>e8e38b2782d87d3b3fe197555f7abd2a73d218df</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/NWTC_Library</t>
+  </si>
+  <si>
+    <t>v2.09.00</t>
+  </si>
+  <si>
+    <t>efab3d7d0c4314064843ab51d8c5b84ab4f8db03</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/ElastoDyn/</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/ServoDyn</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/FEAMooring</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/IceFloe</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/IceDyn</t>
+  </si>
+  <si>
+    <t>9153ed4036e9ddbdd60e0f50597405c2ba84dff3</t>
+  </si>
+  <si>
+    <t>v1.02.01</t>
+  </si>
+  <si>
+    <t>0936b93d79428a00e93790b82b90235dc52b9c1c</t>
+  </si>
+  <si>
+    <t>b1237c432f65a50caa8a82095e807ced0eae0c6c</t>
   </si>
 </sst>
 </file>
@@ -763,7 +812,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -801,8 +850,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -837,6 +893,11 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -847,13 +908,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -970,14 +1032,27 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -1282,8 +1357,798 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" t="s">
+        <v>156</v>
+      </c>
+      <c r="H10" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="D14" s="49">
+        <v>42472</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="H14" s="18"/>
+      <c r="I14"/>
+      <c r="J14" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="D15" s="49">
+        <v>42468</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="7"/>
+      <c r="H15" s="18"/>
+      <c r="I15"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="D16" s="49">
+        <v>42472</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="H16" s="18"/>
+      <c r="I16"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="34" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>240</v>
+      </c>
+      <c r="D17" s="49">
+        <v>42471</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="H17" s="18"/>
+      <c r="I17"/>
+      <c r="J17" s="20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>236</v>
+      </c>
+      <c r="D18" s="49">
+        <v>42471</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="H18" s="18"/>
+      <c r="I18"/>
+      <c r="J18" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>235</v>
+      </c>
+      <c r="D19" s="49">
+        <v>42471</v>
+      </c>
+      <c r="E19" s="32"/>
+      <c r="F19" s="7"/>
+      <c r="H19" s="18"/>
+      <c r="I19"/>
+      <c r="J19" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="H20" s="18"/>
+      <c r="I20"/>
+      <c r="J20" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="D21" s="49">
+        <v>42471</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="H21" s="18"/>
+      <c r="I21"/>
+      <c r="J21" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="D22" s="49">
+        <v>42440</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="7"/>
+      <c r="H22" s="18"/>
+      <c r="I22"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" s="49">
+        <v>42377</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="H23" s="18"/>
+      <c r="I23"/>
+      <c r="J23" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="K23" s="34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" s="49">
+        <v>42444</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="H24" s="18"/>
+      <c r="I24"/>
+      <c r="J24" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="D25" s="49">
+        <v>42471</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="H25" s="18"/>
+      <c r="I25"/>
+      <c r="J25" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="49">
+        <v>42471</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="H26" s="18"/>
+      <c r="I26"/>
+      <c r="J26" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="D27" s="49">
+        <v>42471</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="H27" s="18"/>
+      <c r="I27"/>
+      <c r="J27" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K27" s="34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>258</v>
+      </c>
+      <c r="D28" s="18">
+        <v>42574</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="H28" s="18">
+        <v>42574</v>
+      </c>
+      <c r="I28" t="s">
+        <v>258</v>
+      </c>
+      <c r="J28" s="31"/>
+      <c r="K28" s="20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>218</v>
+      </c>
+      <c r="D29" s="49">
+        <v>42468</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="H29" s="18"/>
+      <c r="I29"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>234</v>
+      </c>
+      <c r="D30" s="18">
+        <v>42574</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="H30" s="18">
+        <v>42574</v>
+      </c>
+      <c r="I30" t="s">
+        <v>234</v>
+      </c>
+      <c r="J30" s="31"/>
+      <c r="K30" s="20" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="18">
+        <v>42574</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="H31" s="18">
+        <v>42574</v>
+      </c>
+      <c r="I31" t="s">
+        <v>258</v>
+      </c>
+      <c r="J31" s="31"/>
+      <c r="K31" s="20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="46" t="s">
+        <v>250</v>
+      </c>
+      <c r="D32" s="18">
+        <v>42574</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="H32" s="18">
+        <v>42574</v>
+      </c>
+      <c r="I32" t="s">
+        <v>250</v>
+      </c>
+      <c r="J32" s="31"/>
+      <c r="K32" s="20" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="D33" s="18">
+        <v>42574</v>
+      </c>
+      <c r="E33" s="32"/>
+      <c r="F33" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="H33" s="18">
+        <v>42574</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="J33" s="31"/>
+      <c r="K33" s="20" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C34" s="46"/>
+      <c r="E34" s="19"/>
+      <c r="G34" s="46"/>
+      <c r="J34" s="46"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C35" s="46"/>
+      <c r="E35" s="19"/>
+      <c r="G35" s="46"/>
+      <c r="J35" s="46"/>
+    </row>
+    <row r="36" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C38" s="46"/>
+      <c r="E38" s="19"/>
+      <c r="G38" s="46"/>
+      <c r="J38" s="46"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C39" s="46"/>
+      <c r="E39" s="19"/>
+      <c r="G39" s="46"/>
+      <c r="J39" s="46"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C40" s="46"/>
+      <c r="E40" s="19"/>
+      <c r="G40" s="46"/>
+      <c r="J40" s="46"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C41" s="46"/>
+      <c r="E41" s="19"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C42" s="46"/>
+      <c r="E42" s="19"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C43" s="46"/>
+      <c r="E43" s="19"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C44" s="46"/>
+      <c r="E44" s="19"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C45" s="46"/>
+      <c r="E45" s="19"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E46" s="17"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E47" s="17"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E48" s="17"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="B37:K37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K32" r:id="rId1"/>
+    <hyperlink ref="J14" r:id="rId2"/>
+    <hyperlink ref="E18" r:id="rId3"/>
+    <hyperlink ref="E24" r:id="rId4"/>
+    <hyperlink ref="E27" r:id="rId5"/>
+    <hyperlink ref="E32" r:id="rId6"/>
+    <hyperlink ref="E14" r:id="rId7"/>
+    <hyperlink ref="E21" r:id="rId8"/>
+    <hyperlink ref="E26" r:id="rId9"/>
+    <hyperlink ref="K15" r:id="rId10"/>
+    <hyperlink ref="J18" r:id="rId11"/>
+    <hyperlink ref="J24" r:id="rId12"/>
+    <hyperlink ref="J21" r:id="rId13"/>
+    <hyperlink ref="J26" r:id="rId14"/>
+    <hyperlink ref="E1" r:id="rId15"/>
+    <hyperlink ref="E30" r:id="rId16"/>
+    <hyperlink ref="E23" r:id="rId17"/>
+    <hyperlink ref="E28" r:id="rId18"/>
+    <hyperlink ref="E31" r:id="rId19"/>
+    <hyperlink ref="J23" r:id="rId20"/>
+    <hyperlink ref="J27" r:id="rId21"/>
+    <hyperlink ref="K29" r:id="rId22"/>
+    <hyperlink ref="E16" r:id="rId23"/>
+    <hyperlink ref="E25" r:id="rId24"/>
+    <hyperlink ref="E29" r:id="rId25"/>
+    <hyperlink ref="J19" r:id="rId26"/>
+    <hyperlink ref="E17" r:id="rId27"/>
+    <hyperlink ref="J20" r:id="rId28"/>
+    <hyperlink ref="E20" r:id="rId29"/>
+    <hyperlink ref="J25" r:id="rId30"/>
+    <hyperlink ref="K16" r:id="rId31"/>
+    <hyperlink ref="J17" r:id="rId32"/>
+    <hyperlink ref="K22" r:id="rId33"/>
+    <hyperlink ref="K23" r:id="rId34"/>
+    <hyperlink ref="K27" r:id="rId35"/>
+    <hyperlink ref="K33" r:id="rId36"/>
+    <hyperlink ref="G33" r:id="rId37"/>
+    <hyperlink ref="G32" r:id="rId38"/>
+    <hyperlink ref="K28" r:id="rId39"/>
+    <hyperlink ref="K30" r:id="rId40"/>
+    <hyperlink ref="K31" r:id="rId41"/>
+    <hyperlink ref="G30" r:id="rId42"/>
+    <hyperlink ref="G31" r:id="rId43"/>
+    <hyperlink ref="G28" r:id="rId44"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId45"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1325,11 +2190,11 @@
       <c r="B5" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -1439,18 +2304,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -2066,16 +2931,16 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="47"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C38" s="41"/>
@@ -2178,12 +3043,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2225,11 +3090,11 @@
       <c r="B5" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -2339,18 +3204,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2935,16 +3800,16 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="47"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C38" s="40"/>
@@ -3045,7 +3910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
@@ -3092,11 +3957,11 @@
       <c r="B5" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -3208,18 +4073,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3648,16 +4513,16 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" s="33"/>
@@ -3748,12 +4613,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3794,11 +4659,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -3874,18 +4739,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
@@ -4248,16 +5113,16 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C31" s="14"/>
@@ -4342,7 +5207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
@@ -4388,11 +5253,11 @@
       <c r="B7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -4468,18 +5333,18 @@
       <c r="B12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
@@ -4925,7 +5790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>

</xml_diff>

<commit_message>
fixed potentially bad index if module wasn't being used during linearization updated dependencies with (hopefully final code for release)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1303 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1776" yWindow="6660" windowWidth="11808" windowHeight="3588"/>
+    <workbookView xWindow="1776" yWindow="6720" windowWidth="11808" windowHeight="2964"/>
   </bookViews>
   <sheets>
     <sheet name="FAST v8.16.00" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="278">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -803,6 +803,57 @@
   </si>
   <si>
     <t>b1237c432f65a50caa8a82095e807ced0eae0c6c</t>
+  </si>
+  <si>
+    <t>v14.05.01a-bjj</t>
+  </si>
+  <si>
+    <t>4425fe175436824f7ae70cb49f5c5dae6897a624</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/OrcaFlexInterface</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/AeroDyn14</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/AeroDyn</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/InflowWind</t>
+  </si>
+  <si>
+    <t>v14.05.01</t>
+  </si>
+  <si>
+    <t>7ab2c2b2f951593aa94fd7917b57392e7017fca6</t>
+  </si>
+  <si>
+    <t>Rev/Commit</t>
+  </si>
+  <si>
+    <t>v1.04.00a-bjj</t>
+  </si>
+  <si>
+    <t>v1.01.04</t>
+  </si>
+  <si>
+    <t>v3.03.00</t>
+  </si>
+  <si>
+    <t>d029391a905f40e9f50143ffe0e7eadc8c32e48c</t>
+  </si>
+  <si>
+    <t>v1.06.00a-bjj</t>
+  </si>
+  <si>
+    <t>v15.03.00</t>
+  </si>
+  <si>
+    <t>v2.05.01</t>
+  </si>
+  <si>
+    <t>https://github.com/NWTC/HydroDyn</t>
   </si>
 </sst>
 </file>
@@ -812,7 +863,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,15 +901,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -893,11 +937,6 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -908,12 +947,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1041,18 +1079,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -1357,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1369,7 +1404,7 @@
     <col min="4" max="4" width="11.6640625" style="46" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="46" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5546875" style="46" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="57.5546875" bestFit="1" customWidth="1"/>
@@ -1545,7 +1580,7 @@
         <v>232</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>136</v>
+        <v>269</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>4</v>
@@ -1567,8 +1602,8 @@
       <c r="C14" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="D14" s="49">
-        <v>42472</v>
+      <c r="D14" s="18">
+        <v>42578</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>181</v>
@@ -1584,14 +1619,14 @@
       <c r="B15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="D15" s="49">
-        <v>42468</v>
+      <c r="C15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" s="18">
+        <v>42577</v>
       </c>
       <c r="E15" s="32"/>
-      <c r="F15" s="7"/>
+      <c r="F15" s="49"/>
       <c r="H15" s="18"/>
       <c r="I15"/>
       <c r="J15" s="31"/>
@@ -1603,11 +1638,11 @@
       <c r="B16" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="51" t="s">
-        <v>241</v>
-      </c>
-      <c r="D16" s="49">
-        <v>42472</v>
+      <c r="C16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="18">
+        <v>42577</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>205</v>
@@ -1615,8 +1650,7 @@
       <c r="F16" s="7"/>
       <c r="H16" s="18"/>
       <c r="I16"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="34" t="s">
+      <c r="J16" s="34" t="s">
         <v>200</v>
       </c>
     </row>
@@ -1624,11 +1658,11 @@
       <c r="B17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="51" t="s">
-        <v>240</v>
-      </c>
-      <c r="D17" s="49">
-        <v>42471</v>
+      <c r="C17" t="s">
+        <v>275</v>
+      </c>
+      <c r="D17" s="18">
+        <v>42578</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>206</v>
@@ -1636,46 +1670,57 @@
       <c r="F17" s="7"/>
       <c r="H17" s="18"/>
       <c r="I17"/>
-      <c r="J17" s="20" t="s">
-        <v>202</v>
+      <c r="J17" s="31"/>
+      <c r="K17" s="34" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C18" s="51" t="s">
-        <v>236</v>
-      </c>
-      <c r="D18" s="49">
-        <v>42471</v>
+      <c r="C18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18" s="18">
+        <v>42576</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>207</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="H18" s="18"/>
-      <c r="I18"/>
-      <c r="J18" s="20" t="s">
-        <v>53</v>
+      <c r="G18" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="H18" s="18">
+        <v>42576</v>
+      </c>
+      <c r="I18" t="s">
+        <v>267</v>
+      </c>
+      <c r="J18" s="31"/>
+      <c r="K18" s="34" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" t="s">
         <v>235</v>
       </c>
-      <c r="D19" s="49">
+      <c r="D19" s="18">
         <v>42471</v>
       </c>
       <c r="E19" s="32"/>
-      <c r="F19" s="7"/>
-      <c r="H19" s="18"/>
-      <c r="I19"/>
-      <c r="J19" s="20" t="s">
-        <v>53</v>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="34" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
@@ -1683,49 +1728,61 @@
         <v>179</v>
       </c>
       <c r="C20" s="32"/>
-      <c r="D20" s="50"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="H20" s="18"/>
-      <c r="I20"/>
-      <c r="J20" s="20" t="s">
-        <v>180</v>
+      <c r="F20" s="45"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="34" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="51" t="s">
-        <v>233</v>
-      </c>
-      <c r="D21" s="49">
-        <v>42471</v>
+      <c r="C21" t="s">
+        <v>272</v>
+      </c>
+      <c r="D21" s="18">
+        <v>42577</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="H21" s="18"/>
-      <c r="I21"/>
-      <c r="J21" s="20" t="s">
-        <v>161</v>
+      <c r="F21" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="H21" s="18">
+        <v>42577</v>
+      </c>
+      <c r="I21" t="s">
+        <v>272</v>
+      </c>
+      <c r="J21" s="31"/>
+      <c r="K21" s="34" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="51" t="s">
-        <v>229</v>
-      </c>
-      <c r="D22" s="49">
-        <v>42440</v>
+      <c r="C22" t="s">
+        <v>274</v>
+      </c>
+      <c r="D22" s="18">
+        <v>42577</v>
       </c>
       <c r="E22" s="32"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="49"/>
       <c r="H22" s="18"/>
       <c r="I22"/>
       <c r="J22" s="31"/>
@@ -1737,21 +1794,22 @@
       <c r="B23" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" t="s">
         <v>225</v>
       </c>
-      <c r="D23" s="49">
+      <c r="D23" s="18">
         <v>42377</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="H23" s="18"/>
-      <c r="I23"/>
-      <c r="J23" s="20" t="s">
-        <v>130</v>
-      </c>
+      <c r="F23" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="G23" s="51"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="31"/>
       <c r="K23" s="34" t="s">
         <v>253</v>
       </c>
@@ -1760,11 +1818,11 @@
       <c r="B24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" s="49">
-        <v>42444</v>
+      <c r="C24" t="s">
+        <v>276</v>
+      </c>
+      <c r="D24" s="18">
+        <v>42578</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>210</v>
@@ -1772,38 +1830,49 @@
       <c r="F24" s="7"/>
       <c r="H24" s="18"/>
       <c r="I24"/>
-      <c r="J24" s="20" t="s">
-        <v>97</v>
+      <c r="J24" s="31"/>
+      <c r="K24" s="34" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="C25" s="51" t="s">
-        <v>234</v>
-      </c>
-      <c r="D25" s="49">
-        <v>42471</v>
+      <c r="C25" t="s">
+        <v>217</v>
+      </c>
+      <c r="D25" s="18">
+        <v>42576</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="H25" s="18"/>
-      <c r="I25"/>
-      <c r="J25" s="20" t="s">
-        <v>228</v>
+      <c r="F25" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="H25" s="18">
+        <v>42576</v>
+      </c>
+      <c r="I25" t="s">
+        <v>217</v>
+      </c>
+      <c r="J25" s="31"/>
+      <c r="K25" s="34" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" t="s">
         <v>239</v>
       </c>
-      <c r="D26" s="49">
+      <c r="D26" s="18">
         <v>42471</v>
       </c>
       <c r="E26" s="20" t="s">
@@ -1820,18 +1889,27 @@
       <c r="B27" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="C27" t="s">
         <v>230</v>
       </c>
-      <c r="D27" s="49">
+      <c r="D27" s="18">
         <v>42471</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="H27" s="18"/>
-      <c r="I27"/>
+      <c r="F27" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="G27" s="44">
+        <v>132</v>
+      </c>
+      <c r="H27" s="50">
+        <v>42471</v>
+      </c>
+      <c r="I27" s="50" t="s">
+        <v>238</v>
+      </c>
       <c r="J27" s="20" t="s">
         <v>42</v>
       </c>
@@ -1871,18 +1949,27 @@
       <c r="B29" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C29" t="s">
         <v>218</v>
       </c>
-      <c r="D29" s="49">
+      <c r="D29" s="18">
         <v>42468</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="H29" s="18"/>
-      <c r="I29"/>
+      <c r="F29" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="G29" s="44">
+        <v>85</v>
+      </c>
+      <c r="H29" s="50">
+        <v>42468</v>
+      </c>
+      <c r="I29" s="44" t="s">
+        <v>218</v>
+      </c>
       <c r="J29" s="31"/>
       <c r="K29" s="34" t="s">
         <v>159</v>
@@ -1901,7 +1988,7 @@
       <c r="E30" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="45" t="s">
         <v>221</v>
       </c>
       <c r="G30" s="34" t="s">
@@ -1931,7 +2018,7 @@
       <c r="E31" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="45" t="s">
         <v>221</v>
       </c>
       <c r="G31" s="34" t="s">
@@ -1989,7 +2076,7 @@
         <v>42574</v>
       </c>
       <c r="E33" s="32"/>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="45" t="s">
         <v>221</v>
       </c>
       <c r="G33" s="34" t="s">
@@ -2103,43 +2190,45 @@
     <hyperlink ref="E21" r:id="rId8"/>
     <hyperlink ref="E26" r:id="rId9"/>
     <hyperlink ref="K15" r:id="rId10"/>
-    <hyperlink ref="J18" r:id="rId11"/>
-    <hyperlink ref="J24" r:id="rId12"/>
-    <hyperlink ref="J21" r:id="rId13"/>
-    <hyperlink ref="J26" r:id="rId14"/>
-    <hyperlink ref="E1" r:id="rId15"/>
-    <hyperlink ref="E30" r:id="rId16"/>
-    <hyperlink ref="E23" r:id="rId17"/>
-    <hyperlink ref="E28" r:id="rId18"/>
-    <hyperlink ref="E31" r:id="rId19"/>
-    <hyperlink ref="J23" r:id="rId20"/>
-    <hyperlink ref="J27" r:id="rId21"/>
-    <hyperlink ref="K29" r:id="rId22"/>
-    <hyperlink ref="E16" r:id="rId23"/>
-    <hyperlink ref="E25" r:id="rId24"/>
-    <hyperlink ref="E29" r:id="rId25"/>
-    <hyperlink ref="J19" r:id="rId26"/>
-    <hyperlink ref="E17" r:id="rId27"/>
-    <hyperlink ref="J20" r:id="rId28"/>
-    <hyperlink ref="E20" r:id="rId29"/>
-    <hyperlink ref="J25" r:id="rId30"/>
-    <hyperlink ref="K16" r:id="rId31"/>
-    <hyperlink ref="J17" r:id="rId32"/>
-    <hyperlink ref="K22" r:id="rId33"/>
-    <hyperlink ref="K23" r:id="rId34"/>
-    <hyperlink ref="K27" r:id="rId35"/>
-    <hyperlink ref="K33" r:id="rId36"/>
-    <hyperlink ref="G33" r:id="rId37"/>
-    <hyperlink ref="G32" r:id="rId38"/>
-    <hyperlink ref="K28" r:id="rId39"/>
-    <hyperlink ref="K30" r:id="rId40"/>
-    <hyperlink ref="K31" r:id="rId41"/>
-    <hyperlink ref="G30" r:id="rId42"/>
-    <hyperlink ref="G31" r:id="rId43"/>
-    <hyperlink ref="G28" r:id="rId44"/>
+    <hyperlink ref="J26" r:id="rId11"/>
+    <hyperlink ref="E1" r:id="rId12"/>
+    <hyperlink ref="E30" r:id="rId13"/>
+    <hyperlink ref="E23" r:id="rId14"/>
+    <hyperlink ref="E28" r:id="rId15"/>
+    <hyperlink ref="E31" r:id="rId16"/>
+    <hyperlink ref="J27" r:id="rId17"/>
+    <hyperlink ref="K29" r:id="rId18"/>
+    <hyperlink ref="E16" r:id="rId19"/>
+    <hyperlink ref="E25" r:id="rId20"/>
+    <hyperlink ref="E29" r:id="rId21"/>
+    <hyperlink ref="E17" r:id="rId22"/>
+    <hyperlink ref="E20" r:id="rId23"/>
+    <hyperlink ref="J16" r:id="rId24"/>
+    <hyperlink ref="K22" r:id="rId25"/>
+    <hyperlink ref="K23" r:id="rId26"/>
+    <hyperlink ref="K27" r:id="rId27"/>
+    <hyperlink ref="K33" r:id="rId28"/>
+    <hyperlink ref="G33" r:id="rId29"/>
+    <hyperlink ref="G32" r:id="rId30"/>
+    <hyperlink ref="K28" r:id="rId31"/>
+    <hyperlink ref="K30" r:id="rId32"/>
+    <hyperlink ref="K31" r:id="rId33"/>
+    <hyperlink ref="G30" r:id="rId34"/>
+    <hyperlink ref="G31" r:id="rId35"/>
+    <hyperlink ref="G28" r:id="rId36"/>
+    <hyperlink ref="G25" r:id="rId37"/>
+    <hyperlink ref="K25" r:id="rId38"/>
+    <hyperlink ref="K18" r:id="rId39"/>
+    <hyperlink ref="K17" r:id="rId40"/>
+    <hyperlink ref="K19" r:id="rId41"/>
+    <hyperlink ref="K20" r:id="rId42"/>
+    <hyperlink ref="K21" r:id="rId43"/>
+    <hyperlink ref="G18" r:id="rId44"/>
+    <hyperlink ref="G21" r:id="rId45"/>
+    <hyperlink ref="K24" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId45"/>
+  <pageSetup orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -2148,7 +2237,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="G27" sqref="G27:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated some files for release
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1307 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/Source/dependencies/FAST_dependencies.xlsx
+++ b/Source/dependencies/FAST_dependencies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="285">
   <si>
     <t>FAST Registry</t>
   </si>
@@ -854,6 +854,27 @@
   </si>
   <si>
     <t>https://github.com/NWTC/HydroDyn</t>
+  </si>
+  <si>
+    <t>e8bcb07d48d9b32934af9dad82fab9eeae14c033</t>
+  </si>
+  <si>
+    <t>4b9b84b50373bb0132ee93d3b365cc69779d8f09</t>
+  </si>
+  <si>
+    <t>v1.04.00</t>
+  </si>
+  <si>
+    <t>mbc</t>
+  </si>
+  <si>
+    <t>v1.06.00</t>
+  </si>
+  <si>
+    <t>4c0631a118dfe0c92ce46f96a1ec7f75233b1dd0</t>
+  </si>
+  <si>
+    <t>v8.16.00</t>
   </si>
 </sst>
 </file>
@@ -1390,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1609,8 +1630,15 @@
         <v>181</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="H14" s="18"/>
-      <c r="I14"/>
+      <c r="G14">
+        <v>1307</v>
+      </c>
+      <c r="H14" s="18">
+        <v>42578</v>
+      </c>
+      <c r="I14" t="s">
+        <v>284</v>
+      </c>
       <c r="J14" s="20" t="s">
         <v>23</v>
       </c>
@@ -1627,8 +1655,15 @@
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="49"/>
-      <c r="H15" s="18"/>
-      <c r="I15"/>
+      <c r="G15" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="H15" s="18">
+        <v>42577</v>
+      </c>
+      <c r="I15" t="s">
+        <v>280</v>
+      </c>
       <c r="J15" s="31"/>
       <c r="K15" s="20" t="s">
         <v>252</v>
@@ -1667,9 +1702,18 @@
       <c r="E17" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="H17" s="18"/>
-      <c r="I17"/>
+      <c r="F17" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="H17" s="18">
+        <v>42578</v>
+      </c>
+      <c r="I17" t="s">
+        <v>275</v>
+      </c>
       <c r="J17" s="31"/>
       <c r="K17" s="34" t="s">
         <v>265</v>
@@ -1783,8 +1827,15 @@
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="49"/>
-      <c r="H22" s="18"/>
-      <c r="I22"/>
+      <c r="G22" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="H22" s="18">
+        <v>42577</v>
+      </c>
+      <c r="I22" t="s">
+        <v>282</v>
+      </c>
       <c r="J22" s="31"/>
       <c r="K22" s="34" t="s">
         <v>253</v>
@@ -1878,9 +1929,18 @@
       <c r="E26" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="H26" s="18"/>
-      <c r="I26"/>
+      <c r="F26" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="G26" s="44">
+        <v>368</v>
+      </c>
+      <c r="H26" s="50">
+        <v>42471</v>
+      </c>
+      <c r="I26" s="50" t="s">
+        <v>239</v>
+      </c>
       <c r="J26" s="20" t="s">
         <v>98</v>
       </c>
@@ -2094,10 +2154,18 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="13" t="s">
+        <v>281</v>
+      </c>
       <c r="C34" s="46"/>
-      <c r="E34" s="19"/>
-      <c r="G34" s="46"/>
-      <c r="J34" s="46"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="20"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C35" s="46"/>
@@ -2105,28 +2173,28 @@
       <c r="G35" s="46"/>
       <c r="J35" s="46"/>
     </row>
-    <row r="36" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C36" s="46"/>
+      <c r="E36" s="19"/>
+      <c r="G36" s="46"/>
+      <c r="J36" s="46"/>
+    </row>
+    <row r="37" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="36" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-    </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C38" s="46"/>
-      <c r="E38" s="19"/>
-      <c r="G38" s="46"/>
-      <c r="J38" s="46"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C39" s="46"/>
@@ -2143,6 +2211,8 @@
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C41" s="46"/>
       <c r="E41" s="19"/>
+      <c r="G41" s="46"/>
+      <c r="J41" s="46"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C42" s="46"/>
@@ -2161,7 +2231,8 @@
       <c r="E45" s="19"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E46" s="17"/>
+      <c r="C46" s="46"/>
+      <c r="E46" s="19"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E47" s="17"/>
@@ -2171,13 +2242,16 @@
     </row>
     <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="17"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="G12:J12"/>
-    <mergeCell ref="B37:K37"/>
+    <mergeCell ref="B38:K38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K32" r:id="rId1"/>
@@ -2226,9 +2300,12 @@
     <hyperlink ref="G18" r:id="rId44"/>
     <hyperlink ref="G21" r:id="rId45"/>
     <hyperlink ref="K24" r:id="rId46"/>
+    <hyperlink ref="G17" r:id="rId47"/>
+    <hyperlink ref="G15" r:id="rId48"/>
+    <hyperlink ref="G22" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId47"/>
+  <pageSetup orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
 
@@ -2237,7 +2314,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:I27"/>
+      <selection activeCell="G26" sqref="G26:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>